<commit_message>
Limits the record number for tests at max data length
</commit_message>
<xml_diff>
--- a/test/datasource.xlsx
+++ b/test/datasource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\zephyrin\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98688D3C-83CF-4258-A02A-B83349FE4AD6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{686F29D3-382D-49C2-BC26-EC5E67155B63}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16386" windowHeight="8190" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="8">
   <si>
     <t>email</t>
   </si>
@@ -44,12 +44,18 @@
   <si>
     <t>pascal.fluck@pfcomputing.ch</t>
   </si>
+  <si>
+    <t>paf18@enigme.ch</t>
+  </si>
+  <si>
+    <t>taratta la patate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -58,6 +64,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -79,14 +92,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -902,8 +918,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" s="1" t="s">
-        <v>4</v>
+      <c r="A36" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -911,8 +927,8 @@
       <c r="C36">
         <v>1034</v>
       </c>
-      <c r="D36">
-        <v>5034</v>
+      <c r="D36" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>